<commit_message>
Final commit with recordings and .bat file
</commit_message>
<xml_diff>
--- a/testData/FindingHospitals_TestData.xlsx
+++ b/testData/FindingHospitals_TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="14">
   <si>
     <t>CityName</t>
   </si>
@@ -551,7 +551,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">

</xml_diff>